<commit_message>
Proftaak, puntjes op de i aan het zetten
</commit_message>
<xml_diff>
--- a/documents/WBSproftaak.xlsx
+++ b/documents/WBSproftaak.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damia\Dropbox\@A_proftaak\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Desktop\USBWEB\root\Proftaak-biocodegaming-web\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>

</xml_diff>